<commit_message>
Fixed the issue Alla pointed out on preqs
There was a section of code commented out that needed to be uncommented
for scanPrereqs
</commit_message>
<xml_diff>
--- a/TestFiles/prerequisites/SQASignOff-PREREQUISTES.xlsx
+++ b/TestFiles/prerequisites/SQASignOff-PREREQUISTES.xlsx
@@ -174,13 +174,13 @@
     <t>PASS</t>
   </si>
   <si>
-    <t>FAIL</t>
-  </si>
-  <si>
-    <t>SCANNER DID NOT CATCH THE ERROR</t>
-  </si>
-  <si>
-    <t>line 12 input accepted</t>
+    <t>SCANNER DID NOT CATCH THE ERROR  (FIXED ON 4/23 BY JARED COX)</t>
+  </si>
+  <si>
+    <t>FAIL(PASS NOW)</t>
+  </si>
+  <si>
+    <t>line 12 input accepted (FIXED ON 4/23 BY JARED COX)</t>
   </si>
 </sst>
 </file>
@@ -568,8 +568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -787,7 +787,7 @@
       </c>
       <c r="E14" s="3"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>18</v>
       </c>
@@ -797,11 +797,11 @@
       <c r="C15" s="4">
         <v>41386</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -909,7 +909,7 @@
       </c>
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>26</v>
       </c>
@@ -919,10 +919,10 @@
       <c r="C23" s="4">
         <v>41386</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E23" s="3" t="s">
+      <c r="D23" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>